<commit_message>
Bumped hitter replacement level
</commit_message>
<xml_diff>
--- a/replacement/replacement_hitters.xlsx
+++ b/replacement/replacement_hitters.xlsx
@@ -1,32 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\replacement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6B802433-8DD4-4929-AEF3-7F2750044554}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBCD4D8-1F29-4309-9C7A-735180AC1DFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="replacement_hitters" sheetId="1" r:id="rId1"/>
-    <sheet name="C" sheetId="2" r:id="rId2"/>
-    <sheet name="1B" sheetId="3" r:id="rId3"/>
-    <sheet name="2b" sheetId="4" r:id="rId4"/>
-    <sheet name="ss" sheetId="5" r:id="rId5"/>
-    <sheet name="3b" sheetId="6" r:id="rId6"/>
-    <sheet name="OF" sheetId="7" r:id="rId7"/>
+    <sheet name="replacement_hitters" sheetId="8" r:id="rId1"/>
+    <sheet name="unadjusted_replacement_hitters" sheetId="1" r:id="rId2"/>
+    <sheet name="C" sheetId="2" r:id="rId3"/>
+    <sheet name="1B" sheetId="3" r:id="rId4"/>
+    <sheet name="2b" sheetId="4" r:id="rId5"/>
+    <sheet name="ss" sheetId="5" r:id="rId6"/>
+    <sheet name="3b" sheetId="6" r:id="rId7"/>
+    <sheet name="OF" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="120">
   <si>
     <t>Position</t>
   </si>
@@ -371,6 +379,21 @@
   </si>
   <si>
     <t>Chad Pinder</t>
+  </si>
+  <si>
+    <t>Adjustment</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>rbi</t>
+  </si>
+  <si>
+    <t>sb</t>
+  </si>
+  <si>
+    <t>avg</t>
   </si>
 </sst>
 </file>
@@ -1210,11 +1233,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B343557C-54D1-41CA-A08D-38B8F7D860D1}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,19 +1267,24 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>14.181818181818182</v>
+        <f>+unadjusted_replacement_hitters!B2+unadjusted_replacement_hitters!I2</f>
+        <v>21.18181818181818</v>
       </c>
       <c r="C2">
-        <v>4.1818181818181817</v>
+        <f>+unadjusted_replacement_hitters!C2+unadjusted_replacement_hitters!J2</f>
+        <v>7.1818181818181817</v>
       </c>
       <c r="D2">
-        <v>15.090909090909092</v>
+        <f>+unadjusted_replacement_hitters!D2+unadjusted_replacement_hitters!K2</f>
+        <v>22.090909090909093</v>
       </c>
       <c r="E2">
-        <v>0.72727272727272729</v>
+        <f>+unadjusted_replacement_hitters!E2+unadjusted_replacement_hitters!L2</f>
+        <v>2.2272727272727275</v>
       </c>
       <c r="F2">
-        <v>0.23100000000000004</v>
+        <f>+unadjusted_replacement_hitters!F2+unadjusted_replacement_hitters!M2</f>
+        <v>0.25100000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1264,19 +1292,24 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>36.083333333333336</v>
+        <f>+unadjusted_replacement_hitters!B3+unadjusted_replacement_hitters!I3</f>
+        <v>38.083333333333336</v>
       </c>
       <c r="C3">
-        <v>11.833333333333334</v>
+        <f>+unadjusted_replacement_hitters!C3+unadjusted_replacement_hitters!J3</f>
+        <v>12.833333333333334</v>
       </c>
       <c r="D3">
-        <v>39.75</v>
+        <f>+unadjusted_replacement_hitters!D3+unadjusted_replacement_hitters!K3</f>
+        <v>41.75</v>
       </c>
       <c r="E3">
-        <v>1.9166666666666667</v>
+        <f>+unadjusted_replacement_hitters!E3+unadjusted_replacement_hitters!L3</f>
+        <v>2.416666666666667</v>
       </c>
       <c r="F3">
-        <v>0.23716666666666666</v>
+        <f>+unadjusted_replacement_hitters!F3+unadjusted_replacement_hitters!M3</f>
+        <v>0.24216666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1284,19 +1317,24 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>40.545454545454547</v>
+        <f>+unadjusted_replacement_hitters!B4+unadjusted_replacement_hitters!I4</f>
+        <v>43.545454545454547</v>
       </c>
       <c r="C4">
-        <v>8.7272727272727266</v>
+        <f>+unadjusted_replacement_hitters!C4+unadjusted_replacement_hitters!J4</f>
+        <v>10.227272727272727</v>
       </c>
       <c r="D4">
-        <v>37.909090909090907</v>
+        <f>+unadjusted_replacement_hitters!D4+unadjusted_replacement_hitters!K4</f>
+        <v>40.909090909090907</v>
       </c>
       <c r="E4">
-        <v>5.5454545454545459</v>
+        <f>+unadjusted_replacement_hitters!E4+unadjusted_replacement_hitters!L4</f>
+        <v>6.5454545454545459</v>
       </c>
       <c r="F4">
-        <v>0.2463636363636364</v>
+        <f>+unadjusted_replacement_hitters!F4+unadjusted_replacement_hitters!M4</f>
+        <v>0.2563636363636364</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1304,19 +1342,24 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>34.454545454545453</v>
+        <f>+unadjusted_replacement_hitters!B5+unadjusted_replacement_hitters!I5</f>
+        <v>37.454545454545453</v>
       </c>
       <c r="C5">
-        <v>7.4545454545454541</v>
+        <f>+unadjusted_replacement_hitters!C5+unadjusted_replacement_hitters!J5</f>
+        <v>8.9545454545454533</v>
       </c>
       <c r="D5">
-        <v>33.636363636363633</v>
+        <f>+unadjusted_replacement_hitters!D5+unadjusted_replacement_hitters!K5</f>
+        <v>36.636363636363633</v>
       </c>
       <c r="E5">
-        <v>4.5454545454545459</v>
+        <f>+unadjusted_replacement_hitters!E5+unadjusted_replacement_hitters!L5</f>
+        <v>5.5454545454545459</v>
       </c>
       <c r="F5">
-        <v>0.24527272727272731</v>
+        <f>+unadjusted_replacement_hitters!F5+unadjusted_replacement_hitters!M5</f>
+        <v>0.25527272727272732</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1324,19 +1367,24 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>34.25</v>
+        <f>+unadjusted_replacement_hitters!B6+unadjusted_replacement_hitters!I6</f>
+        <v>36.25</v>
       </c>
       <c r="C6">
-        <v>9.3125</v>
+        <f>+unadjusted_replacement_hitters!C6+unadjusted_replacement_hitters!J6</f>
+        <v>10.3125</v>
       </c>
       <c r="D6">
-        <v>35.5</v>
+        <f>+unadjusted_replacement_hitters!D6+unadjusted_replacement_hitters!K6</f>
+        <v>37.5</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <f>+unadjusted_replacement_hitters!E6+unadjusted_replacement_hitters!L6</f>
+        <v>3.5</v>
       </c>
       <c r="F6">
-        <v>0.24974999999999997</v>
+        <f>+unadjusted_replacement_hitters!F6+unadjusted_replacement_hitters!M6</f>
+        <v>0.25474999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1344,24 +1392,24 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <f>AVERAGE(B4:B5)</f>
-        <v>37.5</v>
+        <f>+unadjusted_replacement_hitters!B7+unadjusted_replacement_hitters!I7</f>
+        <v>40.5</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:F7" si="0">AVERAGE(C4:C5)</f>
-        <v>8.0909090909090899</v>
+        <f>+unadjusted_replacement_hitters!C7+unadjusted_replacement_hitters!J7</f>
+        <v>9.5909090909090899</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>35.772727272727266</v>
+        <f>+unadjusted_replacement_hitters!D7+unadjusted_replacement_hitters!K7</f>
+        <v>38.772727272727266</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>5.0454545454545459</v>
+        <f>+unadjusted_replacement_hitters!E7+unadjusted_replacement_hitters!L7</f>
+        <v>6.0454545454545459</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0.24581818181818185</v>
+        <f>+unadjusted_replacement_hitters!F7+unadjusted_replacement_hitters!M7</f>
+        <v>0.25581818181818183</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1369,24 +1417,24 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <f>AVERAGE(B6,B3)</f>
-        <v>35.166666666666671</v>
+        <f>+unadjusted_replacement_hitters!B8+unadjusted_replacement_hitters!I8</f>
+        <v>37.166666666666671</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:F8" si="1">AVERAGE(C6,C3)</f>
-        <v>10.572916666666668</v>
+        <f>+unadjusted_replacement_hitters!C8+unadjusted_replacement_hitters!J8</f>
+        <v>11.572916666666668</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>37.625</v>
+        <f>+unadjusted_replacement_hitters!D8+unadjusted_replacement_hitters!K8</f>
+        <v>39.625</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
-        <v>2.4583333333333335</v>
+        <f>+unadjusted_replacement_hitters!E8+unadjusted_replacement_hitters!L8</f>
+        <v>2.9583333333333335</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
-        <v>0.24345833333333333</v>
+        <f>+unadjusted_replacement_hitters!F8+unadjusted_replacement_hitters!M8</f>
+        <v>0.24845833333333334</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1394,19 +1442,24 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>30.916666666666668</v>
+        <f>+unadjusted_replacement_hitters!B9+unadjusted_replacement_hitters!I9</f>
+        <v>32.916666666666671</v>
       </c>
       <c r="C9">
-        <v>7.5</v>
+        <f>+unadjusted_replacement_hitters!C9+unadjusted_replacement_hitters!J9</f>
+        <v>8.5</v>
       </c>
       <c r="D9">
-        <v>30.75</v>
+        <f>+unadjusted_replacement_hitters!D9+unadjusted_replacement_hitters!K9</f>
+        <v>32.75</v>
       </c>
       <c r="E9">
-        <v>5.916666666666667</v>
+        <f>+unadjusted_replacement_hitters!E9+unadjusted_replacement_hitters!L9</f>
+        <v>6.416666666666667</v>
       </c>
       <c r="F9">
-        <v>0.24249999999999994</v>
+        <f>+unadjusted_replacement_hitters!F9+unadjusted_replacement_hitters!M9</f>
+        <v>0.24749999999999994</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1414,24 +1467,24 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <f>AVERAGE(B2:B9)</f>
-        <v>32.887310606060609</v>
+        <f>+unadjusted_replacement_hitters!B10+unadjusted_replacement_hitters!I10</f>
+        <v>34.887310606060609</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:F10" si="2">AVERAGE(C2:C9)</f>
-        <v>8.4591619318181817</v>
+        <f>+unadjusted_replacement_hitters!C10+unadjusted_replacement_hitters!J10</f>
+        <v>9.4591619318181817</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
-        <v>33.25426136363636</v>
+        <f>+unadjusted_replacement_hitters!D10+unadjusted_replacement_hitters!K10</f>
+        <v>35.25426136363636</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
-        <v>3.6444128787878789</v>
+        <f>+unadjusted_replacement_hitters!E10+unadjusted_replacement_hitters!L10</f>
+        <v>4.1444128787878789</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
-        <v>0.2426661931818182</v>
+        <f>+unadjusted_replacement_hitters!F10+unadjusted_replacement_hitters!M10</f>
+        <v>0.24766619318181821</v>
       </c>
     </row>
   </sheetData>
@@ -1440,6 +1493,389 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>14.181818181818182</v>
+      </c>
+      <c r="C2">
+        <v>4.1818181818181817</v>
+      </c>
+      <c r="D2">
+        <v>15.090909090909092</v>
+      </c>
+      <c r="E2">
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="F2">
+        <v>0.23100000000000004</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>1.5</v>
+      </c>
+      <c r="M2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>36.083333333333336</v>
+      </c>
+      <c r="C3">
+        <v>11.833333333333334</v>
+      </c>
+      <c r="D3">
+        <v>39.75</v>
+      </c>
+      <c r="E3">
+        <v>1.9166666666666667</v>
+      </c>
+      <c r="F3">
+        <v>0.23716666666666666</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>0.5</v>
+      </c>
+      <c r="M3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>40.545454545454547</v>
+      </c>
+      <c r="C4">
+        <v>8.7272727272727266</v>
+      </c>
+      <c r="D4">
+        <v>37.909090909090907</v>
+      </c>
+      <c r="E4">
+        <v>5.5454545454545459</v>
+      </c>
+      <c r="F4">
+        <v>0.2463636363636364</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>1.5</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>34.454545454545453</v>
+      </c>
+      <c r="C5">
+        <v>7.4545454545454541</v>
+      </c>
+      <c r="D5">
+        <v>33.636363636363633</v>
+      </c>
+      <c r="E5">
+        <v>4.5454545454545459</v>
+      </c>
+      <c r="F5">
+        <v>0.24527272727272731</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>1.5</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>34.25</v>
+      </c>
+      <c r="C6">
+        <v>9.3125</v>
+      </c>
+      <c r="D6">
+        <v>35.5</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>0.24974999999999997</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>0.5</v>
+      </c>
+      <c r="M6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <f>AVERAGE(B4:B5)</f>
+        <v>37.5</v>
+      </c>
+      <c r="C7">
+        <f>AVERAGE(C4:C5)</f>
+        <v>8.0909090909090899</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="C7:F7" si="0">AVERAGE(D4:D5)</f>
+        <v>35.772727272727266</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>5.0454545454545459</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.24581818181818185</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>1.5</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(B6,B3)</f>
+        <v>35.166666666666671</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:F8" si="1">AVERAGE(C6,C3)</f>
+        <v>10.572916666666668</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>37.625</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>2.4583333333333335</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.24345833333333333</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>0.5</v>
+      </c>
+      <c r="M8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>30.916666666666668</v>
+      </c>
+      <c r="C9">
+        <v>7.5</v>
+      </c>
+      <c r="D9">
+        <v>30.75</v>
+      </c>
+      <c r="E9">
+        <v>5.916666666666667</v>
+      </c>
+      <c r="F9">
+        <v>0.24249999999999994</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>0.5</v>
+      </c>
+      <c r="M9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <f>AVERAGE(B2:B9)</f>
+        <v>32.887310606060609</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:F10" si="2">AVERAGE(C2:C9)</f>
+        <v>8.4591619318181817</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>33.25426136363636</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>3.6444128787878789</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>0.2426661931818182</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>0.5</v>
+      </c>
+      <c r="M10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -1752,7 +2188,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -2088,7 +2524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -2401,7 +2837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -2711,7 +3147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -3187,7 +3623,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>

</xml_diff>